<commit_message>
Merged PR 65472: Added TCs [252686, 252691]
Added TCs [252686, 252691]

Related work items: #252686, #252691, #672034
</commit_message>
<xml_diff>
--- a/West.EnterpriseUX.Automation/West.EnterpriseUX.Automation.MobileNew/TestData/DEV/FilterData.xlsx
+++ b/West.EnterpriseUX.Automation/West.EnterpriseUX.Automation.MobileNew/TestData/DEV/FilterData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patilg\source\repos\UAT_Test\EnterpriseUX.MobileAutomation\West.EnterpriseUX.Automation\West.EnterpriseUX.Automation.MobileNew\TestData\DVV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patilg\source\repos\UAT_Test\EnterpriseUX.MobileAutomation\West.EnterpriseUX.Automation\West.EnterpriseUX.Automation.MobileNew\TestData\DEV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7847773E-F5A6-4CD6-81CF-85A6807A9A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBCF0D84-2E2A-4594-9877-BB3E602AEF38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,7 +72,7 @@
     <t>Sales Document Type ID</t>
   </si>
   <si>
-    <t>Equal</t>
+    <t>Does Not Contains</t>
   </si>
 </sst>
 </file>
@@ -392,9 +392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -405,7 +403,7 @@
     <col min="5" max="5" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.6328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.26953125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -455,7 +453,7 @@
         <v>13</v>
       </c>
       <c r="F2">
-        <v>233</v>
+        <v>23</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>

</xml_diff>